<commit_message>
Renamed Lable Tun.lsl Generalise Tun Contents for MT + Kettle
</commit_message>
<xml_diff>
--- a/Brewery/Brewery Parts.xlsx
+++ b/Brewery/Brewery Parts.xlsx
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="58">
   <si>
     <t>Part</t>
   </si>
@@ -173,40 +173,61 @@
     <t>Lots</t>
   </si>
   <si>
-    <t>Label Tun</t>
-  </si>
-  <si>
-    <t>!Animate Brewery</t>
-  </si>
-  <si>
     <t>Add script while whole brewery selected</t>
   </si>
   <si>
     <t>Mash Tun</t>
   </si>
   <si>
-    <t>Animate Mill</t>
-  </si>
-  <si>
-    <t>Animate HLT Lid</t>
-  </si>
-  <si>
-    <t>Animate MT Lid</t>
-  </si>
-  <si>
-    <t>Animate MT Contents</t>
-  </si>
-  <si>
-    <t>Animate Kettle Lid</t>
-  </si>
-  <si>
-    <t>Make these one script and comment out/in lists of processes</t>
-  </si>
-  <si>
     <t>How do we reverse the flow?</t>
   </si>
   <si>
     <t>Chimney</t>
+  </si>
+  <si>
+    <t>Tun Lid</t>
+  </si>
+  <si>
+    <t>Brewery</t>
+  </si>
+  <si>
+    <t>HLT Steam</t>
+  </si>
+  <si>
+    <t>Tun Contents</t>
+  </si>
+  <si>
+    <t>Pump Assembly 1</t>
+  </si>
+  <si>
+    <t>Pump Assembly 2</t>
+  </si>
+  <si>
+    <t>Hot Liquor Tank</t>
+  </si>
+  <si>
+    <t>Label Object from Desc</t>
+  </si>
+  <si>
+    <t>Pump Assembly 1
+Label Obect from Desc</t>
+  </si>
+  <si>
+    <t>Pump Assembly 2
+Label Object from Desc</t>
+  </si>
+  <si>
+    <t>Chiller circuit
+Label Object from Desc</t>
+  </si>
+  <si>
+    <t>add puffer to top</t>
+  </si>
+  <si>
+    <t>Grain/Mash ??</t>
+  </si>
+  <si>
+    <t>Differentiate grain to mash?</t>
   </si>
 </sst>
 </file>
@@ -235,12 +256,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -255,11 +282,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,16 +585,16 @@
   <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="6.140625" bestFit="1" customWidth="1"/>
@@ -613,13 +641,13 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G2" t="s">
         <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -647,7 +675,7 @@
         <v>10</v>
       </c>
       <c r="E4" t="s">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
         <v>37</v>
@@ -660,11 +688,14 @@
       <c r="B5" t="s">
         <v>13</v>
       </c>
+      <c r="C5" t="s">
+        <v>50</v>
+      </c>
       <c r="D5" t="s">
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -678,10 +709,7 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I6" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -694,6 +722,9 @@
       <c r="D7" t="s">
         <v>13</v>
       </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="8" spans="1:9">
       <c r="A8">
@@ -714,13 +745,13 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" t="s">
         <v>16</v>
       </c>
       <c r="E9" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:9">
@@ -734,10 +765,7 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
-        <v>46</v>
-      </c>
-      <c r="I10" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:9">
@@ -753,6 +781,12 @@
       <c r="E11" t="s">
         <v>47</v>
       </c>
+      <c r="F11" t="s">
+        <v>56</v>
+      </c>
+      <c r="I11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12">
@@ -779,7 +813,7 @@
         <v>19</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" spans="1:9">
@@ -796,10 +830,7 @@
         <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I14" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -812,16 +843,22 @@
       <c r="D15" t="s">
         <v>19</v>
       </c>
+      <c r="E15" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="D16" t="s">
         <v>19</v>
+      </c>
+      <c r="I16" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="30">
@@ -834,11 +871,14 @@
       <c r="D17" t="s">
         <v>34</v>
       </c>
+      <c r="E17" t="s">
+        <v>48</v>
+      </c>
       <c r="F17" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="30">
+    <row r="18" spans="1:9" ht="31.5" customHeight="1">
       <c r="A18">
         <v>17</v>
       </c>
@@ -850,6 +890,9 @@
       </c>
       <c r="D18" t="s">
         <v>34</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>38</v>
@@ -865,11 +908,14 @@
       <c r="D19" t="s">
         <v>35</v>
       </c>
+      <c r="E19" t="s">
+        <v>49</v>
+      </c>
       <c r="F19" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="30">
+    <row r="20" spans="1:9" ht="31.5" customHeight="1">
       <c r="A20">
         <v>19</v>
       </c>
@@ -882,11 +928,14 @@
       <c r="D20" t="s">
         <v>35</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="F20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I20" t="s">
-        <v>50</v>
+      <c r="I20" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="30">
@@ -899,11 +948,14 @@
       <c r="D21" t="s">
         <v>35</v>
       </c>
+      <c r="E21" t="s">
+        <v>49</v>
+      </c>
       <c r="F21" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I21" t="s">
-        <v>50</v>
+      <c r="I21" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="30">
@@ -916,11 +968,14 @@
       <c r="D22" t="s">
         <v>36</v>
       </c>
+      <c r="E22" t="s">
+        <v>36</v>
+      </c>
       <c r="F22" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="30">
+    <row r="23" spans="1:9" ht="29.25" customHeight="1">
       <c r="A23">
         <v>22</v>
       </c>
@@ -932,6 +987,9 @@
       </c>
       <c r="D23" t="s">
         <v>36</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>54</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>38</v>
@@ -945,6 +1003,9 @@
         <v>31</v>
       </c>
       <c r="D24" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" t="s">
         <v>36</v>
       </c>
       <c r="F24" s="1" t="s">

</xml_diff>